<commit_message>
feat: OM apointment updated
</commit_message>
<xml_diff>
--- a/05 - WorkedHourPointing/02 - OM's/ApontamentoFrança.xlsx
+++ b/05 - WorkedHourPointing/02 - OM's/ApontamentoFrança.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\05 - WorkedHourPointing\02 - OM's\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C61F161-840B-4265-9E89-A1544EA19695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56945384-0397-4DAF-9F5B-7B734F4E0E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{929CD599-FE6F-45D1-9902-DEE790AAE293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="15">
   <si>
     <t>H</t>
   </si>
@@ -109,12 +110,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -144,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -164,6 +171,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -502,9 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148AE246-E484-45F8-90E7-699F9ED2F840}">
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1597,4 +1614,1853 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51EC3AA-67EB-458C-9F7D-BFC444965FB2}">
+  <dimension ref="A1:J208"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>685601364160</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J2" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>685601382978</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="11">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J3" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>685601382993</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="11">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J4" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>685601383001</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J5" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>685601383016</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J6" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>685601383021</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="11">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J7" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>685601383099</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J8" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>685601383100</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="11">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J9" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>685601383101</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="11">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J10" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>685601383115</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J11" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>685601383133</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="11">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J12" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>685601383213</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J13" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>685601383299</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="11">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J14" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>685601383301</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="11">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J15" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>685601383302</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J16" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>685601383321</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="11">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J17" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>685601383329</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="11">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J18" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>685601383331</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="11">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J19" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>685601383391</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="11">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J20" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>685601383392</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="11">
+        <v>3</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J21" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>685601383403</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="11">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J22" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>685601383424</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="11">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J23" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>685601383435</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="11">
+        <v>3</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J24" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>685601383436</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="11">
+        <v>3</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J25" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>685601383438</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="11">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J26" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>685601383465</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="11">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J27" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>685601383467</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="11">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J28" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>685601383468</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="11">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="5">
+        <v>6854</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="12">
+        <v>160625</v>
+      </c>
+      <c r="J29" s="5">
+        <v>92906145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>685601383532</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>685601383677</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>685601383707</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>685601383710</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>685601383725</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>685601383734</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>685601383804</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>685601383805</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>685601383980</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>685601384024</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>685601384043</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>685601384044</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>685601384045</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>685601384148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>685601384230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>685601384231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>685601384275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>685601384277</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>685601384278</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>685601384364</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
+        <v>685601384366</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9">
+        <v>685601384368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="9">
+        <v>685601384369</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="9">
+        <v>685601384370</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>685601384372</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
+        <v>685601384375</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
+        <v>685601384377</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>685601384494</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>685601384496</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>685601384532</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>685601384567</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>685601384575</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>685601384578</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
+        <v>685601384587</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
+        <v>685601384588</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
+        <v>685601384622</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
+        <v>685601384676</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
+        <v>685601384731</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
+        <v>685601384820</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
+        <v>685601384821</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
+        <v>685601384822</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="9">
+        <v>685601384823</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
+        <v>685601384824</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
+        <v>685601384827</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="9">
+        <v>685601384828</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
+        <v>685601384829</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="9">
+        <v>685601384879</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
+        <v>685601384990</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="9">
+        <v>685601384991</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="9">
+        <v>685601384992</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="9">
+        <v>685601385070</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="9">
+        <v>685601385071</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
+        <v>685601385178</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="9">
+        <v>685601385222</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="9">
+        <v>685601385225</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="9">
+        <v>685601385227</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="9">
+        <v>685601385305</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
+        <v>685601385306</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="9">
+        <v>685601385308</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="9">
+        <v>685601385309</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="9">
+        <v>685601385337</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="9">
+        <v>685601385362</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="9">
+        <v>685601385363</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="9">
+        <v>685601385364</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="9">
+        <v>685601385365</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="9">
+        <v>685601385366</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="9">
+        <v>685601385367</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="9">
+        <v>685601385368</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="9">
+        <v>685601385369</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="9">
+        <v>685601385370</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="9">
+        <v>685601385372</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="9">
+        <v>685601385373</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="9">
+        <v>685601385374</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="9">
+        <v>685601385376</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="9">
+        <v>685601385377</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="9">
+        <v>685601385430</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="9">
+        <v>685601385443</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="9">
+        <v>685601385586</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="9">
+        <v>685601385587</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="9">
+        <v>685601385589</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="9">
+        <v>685601386361</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="9">
+        <v>685601386364</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="9">
+        <v>685601386899</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="9">
+        <v>685601386901</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="9">
+        <v>685601387008</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="9">
+        <v>685601387054</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="9">
+        <v>685601387055</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="9">
+        <v>685601387056</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="9">
+        <v>685601387158</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="9">
+        <v>685601387160</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="9">
+        <v>685601387186</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="9">
+        <v>685601387247</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="9">
+        <v>685601387249</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="9">
+        <v>685601387332</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="9">
+        <v>685601387354</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="9">
+        <v>685601387355</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="9">
+        <v>685601387361</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="9">
+        <v>685601387376</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="9">
+        <v>685601387401</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="9">
+        <v>685601387405</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="9">
+        <v>685601387406</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="9">
+        <v>685601387407</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="9">
+        <v>685601387534</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="9">
+        <v>685601387546</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="9">
+        <v>685601387547</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="9">
+        <v>685601387625</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="9">
+        <v>685601387626</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="9">
+        <v>685601387628</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="9">
+        <v>685601387629</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="9">
+        <v>685601387630</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="9">
+        <v>685601387631</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="9">
+        <v>685601387633</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="9">
+        <v>685601387635</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="9">
+        <v>685601387638</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="9">
+        <v>685601387639</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="9">
+        <v>685601387640</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="9">
+        <v>685601387643</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="9">
+        <v>685601387645</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="9">
+        <v>685601387729</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="9">
+        <v>685601387786</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="9">
+        <v>685601387816</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="9">
+        <v>685601387817</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="9">
+        <v>685601387827</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="9">
+        <v>685601387829</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="9">
+        <v>685601387830</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="9">
+        <v>685601387831</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="9">
+        <v>685601387835</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="9">
+        <v>685601387841</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="9">
+        <v>685601387843</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="9">
+        <v>685601387844</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="9">
+        <v>685601387845</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="9">
+        <v>685601387879</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="9">
+        <v>685601387880</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="9">
+        <v>685601387894</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="9">
+        <v>685601387918</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="9">
+        <v>685601388006</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="9">
+        <v>685601388143</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="9">
+        <v>685601388158</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="9">
+        <v>685601388160</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="9">
+        <v>685601388256</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="9">
+        <v>685601388257</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="9">
+        <v>685601388329</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="9">
+        <v>685601388330</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="9">
+        <v>685601388339</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="9">
+        <v>685601388401</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="9">
+        <v>685601388627</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="9">
+        <v>685601388659</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="9">
+        <v>685601388661</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="9">
+        <v>685601388736</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="9">
+        <v>685601388768</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="9">
+        <v>685601388798</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="9">
+        <v>685601388805</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="9">
+        <v>685601388865</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="9">
+        <v>685601388871</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="9">
+        <v>685601388909</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="9">
+        <v>685601388933</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="9">
+        <v>685601388934</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="9">
+        <v>685601388935</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="9">
+        <v>685601388974</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="9">
+        <v>685601389039</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="9">
+        <v>685601389042</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="9">
+        <v>685601389075</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="9">
+        <v>685601389094</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="9">
+        <v>685601389216</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="9">
+        <v>685601389525</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="9">
+        <v>685601389595</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="9">
+        <v>685601389596</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="9">
+        <v>685601389607</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="9">
+        <v>685601389665</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="9">
+        <v>685601389683</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="9">
+        <v>685601389686</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="9">
+        <v>685601389688</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="9">
+        <v>685601389690</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="9">
+        <v>685601389718</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="9">
+        <v>685601389719</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="9">
+        <v>685601389778</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="9">
+        <v>685601389779</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="9">
+        <v>685601389848</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>